<commit_message>
model edits - now at better model; have incorporation of effect of temp; still need to write loop for modeling w/ range of temps.
</commit_message>
<xml_diff>
--- a/ddCT2_calcs_from_Flinnmodel_withfractions.xlsx
+++ b/ddCT2_calcs_from_Flinnmodel_withfractions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linzm\Documents\Tate Lab Rotation\Tate_Rotation_Temp_Immunity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3C1EBE5-BD68-4729-9242-D738024790E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A15BFE-A726-4029-A4B9-6D5182D69B13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9960" yWindow="0" windowWidth="8900" windowHeight="10090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>Treatment</t>
   </si>
@@ -52,13 +52,19 @@
   </si>
   <si>
     <t>Fraction of ddCT2 at Topt</t>
+  </si>
+  <si>
+    <t>rate = ddCT2 of treat - noninjected / time; time = 4hr</t>
+  </si>
+  <si>
+    <t>% of optimum rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -70,6 +76,21 @@
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,11 +116,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -426,9 +449,10 @@
     <col min="2" max="2" width="5.6796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6796875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,8 +465,14 @@
       <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -455,8 +485,9 @@
       <c r="D2" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -471,7 +502,7 @@
         <v>97.349797666092456</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -486,7 +517,7 @@
         <v>82.41772301085031</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -501,7 +532,7 @@
         <v>56.00379926604505</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -514,8 +545,16 @@
       <c r="D6" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="E6" s="1">
+        <f>C6-C2/4</f>
+        <v>3.5651503376342504</v>
+      </c>
+      <c r="F6" s="4">
+        <f>100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -529,8 +568,16 @@
         <f>C7/C6*100</f>
         <v>97.198635818838028</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="E7">
+        <f>C7-C3/4</f>
+        <v>3.4646726594454256</v>
+      </c>
+      <c r="F7" s="5">
+        <f>E7/E6*100</f>
+        <v>97.181670654160996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -544,8 +591,16 @@
         <f>C8/C6*100</f>
         <v>67.940382151793116</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="E8">
+        <f>C8-C4/4</f>
+        <v>2.3642495636420318</v>
+      </c>
+      <c r="F8" s="5">
+        <f>E8/E6*100</f>
+        <v>66.315564274658101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -559,8 +614,16 @@
         <f>C9/C6*100</f>
         <v>38.718611085903341</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="E9">
+        <f>C9-C5/4</f>
+        <v>1.3112146451721285</v>
+      </c>
+      <c r="F9" s="5">
+        <f>E9/E6*100</f>
+        <v>36.778663478248149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -573,8 +636,15 @@
       <c r="D10" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="E10" s="1">
+        <f>C10-C2/4</f>
+        <v>21.423161003484118</v>
+      </c>
+      <c r="F10" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -588,8 +658,16 @@
         <f>C11/C10*100</f>
         <v>91.675467448987575</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="E11">
+        <f>C11-C3/4</f>
+        <v>19.617078680449183</v>
+      </c>
+      <c r="F11" s="5">
+        <f>E11/E10*100</f>
+        <v>91.569487235141409</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -603,8 +681,16 @@
         <f>C12/C10*100</f>
         <v>40.328624855547126</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="E12">
+        <f>C12-C4/4</f>
+        <v>8.4712579854150096</v>
+      </c>
+      <c r="F12" s="5">
+        <f>E12/E10*100</f>
+        <v>39.542521218214723</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -617,6 +703,14 @@
       <c r="D13" s="3">
         <f>C13/C10*100</f>
         <v>16.764499366052256</v>
+      </c>
+      <c r="E13">
+        <f>C13-C5/4</f>
+        <v>3.4344801468110515</v>
+      </c>
+      <c r="F13" s="5">
+        <f>E13/E10*100</f>
+        <v>16.031621786591113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed loop for within-host model; deleting unncessary files; renamed some files for consistency
</commit_message>
<xml_diff>
--- a/ddCT2_calcs_from_Flinnmodel_withfractions.xlsx
+++ b/ddCT2_calcs_from_Flinnmodel_withfractions.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linzm\Documents\Tate Lab Rotation\Tate_Rotation_Temp_Immunity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A15BFE-A726-4029-A4B9-6D5182D69B13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B990865-2B97-4FD3-8A4C-040A491AB5C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9960" yWindow="0" windowWidth="8900" windowHeight="10090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="710" windowWidth="8900" windowHeight="10090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>

</xml_diff>